<commit_message>
Created some kind algorith for game2 profit
</commit_message>
<xml_diff>
--- a/Casino Voitonjako.xlsx
+++ b/Casino Voitonjako.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osku0\Desktop\Casino-Prototyyppi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1601396\Desktop\Casino-Prototyyppi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Voitto Algoritmi" sheetId="2" r:id="rId1"/>
+    <sheet name="Game1 Voiton jako" sheetId="2" r:id="rId1"/>
+    <sheet name="Game2 Voiton jako" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="21">
   <si>
     <t>=</t>
   </si>
@@ -60,6 +61,33 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>num4</t>
+  </si>
+  <si>
+    <t>num5</t>
+  </si>
+  <si>
+    <t>Summa</t>
+  </si>
+  <si>
+    <t>Keskiarvo</t>
+  </si>
+  <si>
+    <t>Juokseva summa</t>
+  </si>
+  <si>
+    <t>Määrä</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x0.50</t>
+  </si>
+  <si>
+    <t>x10</t>
   </si>
 </sst>
 </file>
@@ -196,23 +224,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -248,23 +259,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,4 +881,1072 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:AO14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>9</v>
+      </c>
+      <c r="M6">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>9</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6">
+        <v>9</v>
+      </c>
+      <c r="T6">
+        <v>9</v>
+      </c>
+      <c r="U6">
+        <v>9</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA6">
+        <v>9</v>
+      </c>
+      <c r="AB6">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH6" s="1"/>
+      <c r="AI6">
+        <v>9</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <v>8</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <v>8</v>
+      </c>
+      <c r="T7">
+        <v>8</v>
+      </c>
+      <c r="U7">
+        <v>8</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA7">
+        <v>8</v>
+      </c>
+      <c r="AB7">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH7" s="1"/>
+      <c r="AI7">
+        <v>8</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <v>7</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA8">
+        <v>7</v>
+      </c>
+      <c r="AB8">
+        <v>7</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH8" s="1"/>
+      <c r="AI8">
+        <v>7</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>6</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <v>6</v>
+      </c>
+      <c r="T9">
+        <v>6</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>6</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH9" s="1"/>
+      <c r="AI9">
+        <v>6</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>5</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH10" s="1"/>
+      <c r="AI10">
+        <v>5</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>4</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA11">
+        <v>4</v>
+      </c>
+      <c r="AB11">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH11" s="1"/>
+      <c r="AI11">
+        <v>4</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA12">
+        <v>3</v>
+      </c>
+      <c r="AB12">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH12" s="1"/>
+      <c r="AI12">
+        <v>3</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="T13">
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>2</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA13">
+        <v>2</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH13" s="1"/>
+      <c r="AI13">
+        <v>2</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH14" s="1"/>
+      <c r="AI14">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>